<commit_message>
Generate sheet including specifics currencies
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report.xlsx
+++ b/src/Controllers/Sheet/outputs/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Documents\Victor\currency_api\src\Controllers\Sheet\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973A187A-47FD-4B08-BBFB-C13FDAB8BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C176CD-E568-483C-868D-63256C26F8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D9CDE337-A4A4-4202-BDB0-1B9F047ECC56}" activeTab="0"/>
   </bookViews>
@@ -61,6 +61,12 @@
     <t xml:space="preserve">NOK</t>
   </si>
   <si>
+    <t xml:space="preserve">Coroa Sueca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dólar</t>
   </si>
   <si>
@@ -118,6 +124,15 @@
     <t xml:space="preserve">£</t>
   </si>
   <si>
+    <t xml:space="preserve">Novo Sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peso Argentino</t>
   </si>
   <si>
@@ -142,6 +157,12 @@
     <t xml:space="preserve">MXN</t>
   </si>
   <si>
+    <t xml:space="preserve">Peso Uruguaio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UYU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yuan</t>
   </si>
   <si>
@@ -154,10 +175,10 @@
     <t xml:space="preserve">Horário do relatório</t>
   </si>
   <si>
-    <t xml:space="preserve">11/11/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21:29</t>
+    <t xml:space="preserve">06/02/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:34</t>
   </si>
 </sst>
 </file>
@@ -183,14 +204,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font/>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -247,25 +273,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyAlignment="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyAlignment="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyAlignment="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyAlignment="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE66C2D-1CA9-406C-B2E0-06F7FFA9C030}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -592,7 +614,7 @@
     <col min="2" max="4" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="1">
         <v>0</v>
       </c>
@@ -602,531 +624,567 @@
       <c r="C1" t="s" s="1">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>0.83</v>
-      </c>
-      <c r="C2" t="s" s="3">
+      <c r="B2" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="C2" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="C3" t="s" s="3">
+      <c r="B3" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="C3" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="D3" t="s" s="3">
+      <c r="D3" t="s" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s" s="3">
+      <c r="A4" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
-        <v>5.4</v>
-      </c>
-      <c r="C4" t="s" s="3">
+      <c r="B4" s="3">
+        <v>0.58</v>
+      </c>
+      <c r="C4" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="D4" t="s" s="3">
+      <c r="D4" t="s" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="3">
+      <c r="B5" s="3">
+        <v>5.33</v>
+      </c>
+      <c r="C5" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B5" s="4">
-        <v>3.94</v>
-      </c>
-      <c r="C5" t="s" s="3">
+      <c r="D5" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="D5" t="s" s="3">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="3">
+      <c r="A6" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B6" s="4">
-        <v>4.29</v>
-      </c>
-      <c r="C6" t="s" s="3">
+      <c r="B6" s="3">
+        <v>3.77</v>
+      </c>
+      <c r="C6" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="D6" t="s" s="3">
-        <v>11</v>
+      <c r="D6" t="s" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="3">
+      <c r="A7" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B7" s="4">
-        <v>6.18</v>
-      </c>
-      <c r="C7" t="s" s="3">
+      <c r="B7" s="3">
+        <v>4.17</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="D7" t="s" s="3">
+      <c r="D7" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="3">
+      <c r="B8" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="C8" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B8" s="4">
-        <v>5.86</v>
-      </c>
-      <c r="C8" t="s" s="3">
+      <c r="D8" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="D8" t="s" s="3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="3">
+      <c r="B9" s="3">
+        <v>5.76</v>
+      </c>
+      <c r="C9" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B9" s="4">
-        <v>0.0473</v>
-      </c>
-      <c r="C9" t="s" s="3">
+      <c r="D9" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="D9" t="s" s="3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="3">
+      <c r="B10" s="3">
+        <v>0.0463</v>
+      </c>
+      <c r="C10" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="B10" s="4">
-        <v>7.22</v>
-      </c>
-      <c r="C10" t="s" s="3">
+      <c r="D10" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="D10" t="s" s="3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="3">
+      <c r="B11" s="3">
+        <v>7.21</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="B11" s="4">
-        <v>0.054</v>
-      </c>
-      <c r="C11" t="s" s="3">
+      <c r="D11" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="D11" t="s" s="3">
-        <v>11</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="3">
+      <c r="A12" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="B12" s="4">
-        <v>0.0068</v>
-      </c>
-      <c r="C12" t="s" s="3">
+      <c r="B12" s="3">
+        <v>1.39</v>
+      </c>
+      <c r="C12" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="D12" t="s" s="3">
-        <v>11</v>
+      <c r="D12" t="s" s="2">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="3">
-        <v>32</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0.0014</v>
-      </c>
-      <c r="C13" t="s" s="3">
+      <c r="A13" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="D13" t="s" s="3">
-        <v>11</v>
+      <c r="B13" s="3">
+        <v>0.051</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="B14" s="4">
+      <c r="A14" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.0064</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.0013</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3">
         <v>0.26</v>
       </c>
-      <c r="C14" t="s" s="3">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="3">
-        <v>36</v>
-      </c>
-      <c r="B15" s="4">
+      <c r="C16" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3">
         <v>0.84</v>
       </c>
-      <c r="C15" t="s" s="3">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s" s="3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="C17" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s" s="7">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" t="s" s="3">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s" s="3">
-        <v>41</v>
+      <c r="C18" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s" s="6">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s" s="5">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Countries related to each currency added
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report.xlsx
+++ b/src/Controllers/Sheet/outputs/report.xlsx
@@ -46,27 +46,6 @@
     <t>Símbolo</t>
   </si>
   <si>
-    <t xml:space="preserve">Coroa Dinamarquesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DKK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroa Norueguesa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coroa Sueca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dólar</t>
   </si>
   <si>
@@ -88,97 +67,16 @@
     <t xml:space="preserve">CAD</t>
   </si>
   <si>
-    <t xml:space="preserve">Euro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">€</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Franco Suíço</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">¥</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Libra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GBP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">£</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Novo Sol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso Argentino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso Chileno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso Colombiano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso Mexicano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MXN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peso Uruguaio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UYU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yuan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CNY</t>
-  </si>
-  <si>
     <t xml:space="preserve">Data das cotações</t>
   </si>
   <si>
     <t xml:space="preserve">Horário do relatório</t>
   </si>
   <si>
-    <t xml:space="preserve">06/02/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23:34</t>
+    <t xml:space="preserve">12/02/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:48</t>
   </si>
 </sst>
 </file>
@@ -633,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>0.82</v>
+        <v>5.25</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>5</v>
@@ -647,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>0.61</v>
+        <v>3.75</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>8</v>
@@ -661,7 +559,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>0.58</v>
+        <v>4.13</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>10</v>
@@ -671,200 +569,96 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s" s="2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
-        <v>5.33</v>
-      </c>
-      <c r="C5" t="s" s="2">
+      <c r="D6" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="D5" t="s" s="2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" t="s" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s" s="2">
+      <c r="D7" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B6" s="3">
-        <v>3.77</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3">
-        <v>4.17</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>20</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s" s="2">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3">
-        <v>5.76</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>23</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.0463</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>26</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3">
-        <v>7.21</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>29</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3">
-        <v>1.39</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>32</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.051</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.0064</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="B15" s="3">
-        <v>0.0013</v>
-      </c>
-      <c r="C15" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="C16" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="B17" s="3">
-        <v>0.122</v>
-      </c>
-      <c r="C17" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>13</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="B18" s="3">
-        <v>0.84</v>
-      </c>
-      <c r="C18" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>26</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
@@ -875,22 +669,14 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
-      <c r="C20" t="s" s="6">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s" s="5">
-        <v>46</v>
-      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
-      <c r="C21" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s" s="2">
-        <v>48</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>

</xml_diff>

<commit_message>
New domain name set up
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report.xlsx
+++ b/src/Controllers/Sheet/outputs/report.xlsx
@@ -67,16 +67,82 @@
     <t xml:space="preserve">CAD</t>
   </si>
   <si>
+    <t xml:space="preserve">Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">€</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franco Suíço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Libra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">£</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso Argentino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso Chileno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso Colombiano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso Mexicano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yuan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CNY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Data das cotações</t>
   </si>
   <si>
     <t xml:space="preserve">Horário do relatório</t>
   </si>
   <si>
-    <t xml:space="preserve">12/02/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16:48</t>
+    <t xml:space="preserve">04/04/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:35</t>
   </si>
 </sst>
 </file>
@@ -531,7 +597,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>5.25</v>
+        <v>4.6</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>5</v>
@@ -545,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>3.75</v>
+        <v>3.47</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>8</v>
@@ -559,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>4.13</v>
+        <v>3.68</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>10</v>
@@ -569,66 +635,130 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5.04</v>
+      </c>
+      <c r="C5" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" t="s" s="6">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s" s="5">
-        <v>12</v>
+      <c r="A6" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4.96</v>
+      </c>
+      <c r="C6" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="A7" t="s" s="2">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.0374</v>
+      </c>
       <c r="C7" t="s" s="2">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6.03</v>
+      </c>
+      <c r="C8" t="s" s="2">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.041</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.0059</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.0012</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.72</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
@@ -639,14 +769,22 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" t="s" s="6">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s" s="5">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>

</xml_diff>

<commit_message>
Filter currency results endpoints added
</commit_message>
<xml_diff>
--- a/src/Controllers/Sheet/outputs/report.xlsx
+++ b/src/Controllers/Sheet/outputs/report.xlsx
@@ -139,10 +139,10 @@
     <t xml:space="preserve">Horário do relatório</t>
   </si>
   <si>
-    <t xml:space="preserve">04/04/2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20:35</t>
+    <t xml:space="preserve">31/07/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22:46</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="3">
-        <v>4.6</v>
+        <v>5.17</v>
       </c>
       <c r="C2" t="s" s="2">
         <v>5</v>
@@ -611,7 +611,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>3.47</v>
+        <v>3.62</v>
       </c>
       <c r="C3" t="s" s="2">
         <v>8</v>
@@ -625,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>3.68</v>
+        <v>4.04</v>
       </c>
       <c r="C4" t="s" s="2">
         <v>10</v>
@@ -639,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>5.04</v>
+        <v>5.29</v>
       </c>
       <c r="C5" t="s" s="2">
         <v>12</v>
@@ -653,7 +653,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>4.96</v>
+        <v>5.44</v>
       </c>
       <c r="C6" t="s" s="2">
         <v>15</v>
@@ -667,7 +667,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="3">
-        <v>0.0374</v>
+        <v>0.0388</v>
       </c>
       <c r="C7" t="s" s="2">
         <v>18</v>
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="3">
-        <v>6.03</v>
+        <v>6.3</v>
       </c>
       <c r="C8" t="s" s="2">
         <v>21</v>
@@ -695,7 +695,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="3">
-        <v>0.041</v>
+        <v>0.04</v>
       </c>
       <c r="C9" t="s" s="2">
         <v>24</v>
@@ -709,7 +709,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="3">
-        <v>0.0059</v>
+        <v>0.0057</v>
       </c>
       <c r="C10" t="s" s="2">
         <v>26</v>
@@ -737,7 +737,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="3">
-        <v>0.23</v>
+        <v>0.25</v>
       </c>
       <c r="C12" t="s" s="2">
         <v>30</v>
@@ -751,7 +751,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="3">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="C13" t="s" s="2">
         <v>32</v>

</xml_diff>